<commit_message>
fixed data point E69 to the corrext date (4.21 > 4/17)
</commit_message>
<xml_diff>
--- a/data/brewnalysis_test_data.xlsx
+++ b/data/brewnalysis_test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bertille/brewnalysis/brewnalysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Documents\github\brewnalysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054D3D9F-F81E-EE4C-A9E5-4C4D77576250}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05D6114-DA4B-48C9-828B-F5639CB6AC1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="860" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -480,16 +480,16 @@
   <dimension ref="A1:P170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="22" width="21.5" customWidth="1"/>
+    <col min="1" max="22" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,7 +539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -589,7 +589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -618,7 +618,7 @@
         <v>4.43</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -647,7 +647,7 @@
         <v>4.38</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -697,7 +697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -747,7 +747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -776,7 +776,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -805,7 +805,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -855,7 +855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -905,7 +905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -955,7 +955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>4.62</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>22</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>22</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>22</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>22</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>4.59</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>22</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>4.57</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>23</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>23</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>23</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>23</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>23</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>23</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>23</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>23</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>23</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>23</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>23</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>4.3899999999999997</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>23</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>23</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>23</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>23</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>23</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>23</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>23</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>23</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>23</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>23</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>23</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>23</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>23</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>23</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>23</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>23</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>23</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>23</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>23</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>24</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>17</v>
       </c>
       <c r="E69" s="2">
-        <v>43942</v>
+        <v>43938</v>
       </c>
       <c r="F69" s="3">
         <v>0.375</v>
@@ -3729,7 +3729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>24</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>4.51</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>24</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>24</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>24</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>24</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>24</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>24</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>24</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>24</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>24</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>24</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>24</v>
       </c>
@@ -4287,7 +4287,7 @@
         <v>4.74</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>24</v>
       </c>
@@ -4337,7 +4337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>24</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>24</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>24</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>24</v>
       </c>
@@ -4516,7 +4516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>24</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>24</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>24</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>24</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>24</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>24</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>24</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>24</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>24</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>4.7699999999999996</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>24</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>24</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>24</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>24</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>24</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>24</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>24</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>24</v>
       </c>
@@ -5303,7 +5303,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>25</v>
       </c>
@@ -5353,7 +5353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>25</v>
       </c>
@@ -5403,7 +5403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>25</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>25</v>
       </c>
@@ -5503,7 +5503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>25</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>25</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>3.93</v>
       </c>
     </row>
-    <row r="110" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>25</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>25</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>25</v>
       </c>
@@ -5711,7 +5711,7 @@
         <v>4.08</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>25</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>4.13</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>25</v>
       </c>
@@ -5769,7 +5769,7 @@
         <v>4.13</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>25</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>25</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>25</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>25</v>
       </c>
@@ -5948,7 +5948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>25</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>25</v>
       </c>
@@ -6048,7 +6048,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>25</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>25</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>25</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>25</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>25</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>25</v>
       </c>
@@ -6327,7 +6327,7 @@
         <v>4.38</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>25</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>25</v>
       </c>
@@ -6427,7 +6427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>25</v>
       </c>
@@ -6477,7 +6477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>25</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>25</v>
       </c>
@@ -6577,7 +6577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>25</v>
       </c>
@@ -6606,7 +6606,7 @@
         <v>4.3499999999999996</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>25</v>
       </c>
@@ -6656,7 +6656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>25</v>
       </c>
@@ -6706,7 +6706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>25</v>
       </c>
@@ -6735,7 +6735,7 @@
         <v>4.3600000000000003</v>
       </c>
     </row>
-    <row r="136" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>26</v>
       </c>
@@ -6785,7 +6785,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>26</v>
       </c>
@@ -6835,7 +6835,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>26</v>
       </c>
@@ -6885,7 +6885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>26</v>
       </c>
@@ -6914,7 +6914,7 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>26</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>26</v>
       </c>
@@ -6972,7 +6972,7 @@
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>26</v>
       </c>
@@ -7022,7 +7022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>26</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>26</v>
       </c>
@@ -7122,7 +7122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>26</v>
       </c>
@@ -7172,7 +7172,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>26</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>26</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>26</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>26</v>
       </c>
@@ -7372,7 +7372,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>26</v>
       </c>
@@ -7422,7 +7422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>26</v>
       </c>
@@ -7472,7 +7472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>26</v>
       </c>
@@ -7522,7 +7522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>26</v>
       </c>
@@ -7572,7 +7572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>26</v>
       </c>
@@ -7622,7 +7622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>26</v>
       </c>
@@ -7672,7 +7672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="156" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>26</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>26</v>
       </c>
@@ -7772,7 +7772,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>26</v>
       </c>
@@ -7822,7 +7822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>26</v>
       </c>
@@ -7872,7 +7872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>26</v>
       </c>
@@ -7922,7 +7922,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>26</v>
       </c>
@@ -7972,7 +7972,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="162" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>26</v>
       </c>
@@ -8022,7 +8022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>26</v>
       </c>
@@ -8072,7 +8072,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="164" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>26</v>
       </c>
@@ -8122,7 +8122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>26</v>
       </c>
@@ -8172,7 +8172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>26</v>
       </c>
@@ -8222,7 +8222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>26</v>
       </c>
@@ -8272,7 +8272,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>26</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>26</v>
       </c>
@@ -8351,7 +8351,7 @@
         <v>4.18</v>
       </c>
     </row>
-    <row r="170" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>